<commit_message>
poprawki po recenzji #1 od pocz do tabel
</commit_message>
<xml_diff>
--- a/korelacje_pearson_r.xlsx
+++ b/korelacje_pearson_r.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Work/PracaMagPiel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6768D285-BBAF-3644-B218-76B8696E0AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DDD2E9-E639-5542-8CB8-3A482309A0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20660" yWindow="-20080" windowWidth="27640" windowHeight="16940" xr2:uid="{CF6C3CBA-C656-6E4B-8054-BE7576B43076}"/>
+    <workbookView xWindow="18820" yWindow="-21100" windowWidth="27920" windowHeight="19940" xr2:uid="{CF6C3CBA-C656-6E4B-8054-BE7576B43076}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>plec</t>
   </si>
@@ -164,7 +164,127 @@
     <t>Q36dobry_wybor</t>
   </si>
   <si>
-    <t>Q37wspiera_dziecko_piel</t>
+    <t>podyplomowe</t>
+  </si>
+  <si>
+    <t>stan cywilny</t>
+  </si>
+  <si>
+    <t>Q1 staż</t>
+  </si>
+  <si>
+    <t>płeć</t>
+  </si>
+  <si>
+    <t>szkoła</t>
+  </si>
+  <si>
+    <t>Q2 etaty</t>
+  </si>
+  <si>
+    <t>Q3 godz</t>
+  </si>
+  <si>
+    <t>Q4 system</t>
+  </si>
+  <si>
+    <t>Q5 zadowolona</t>
+  </si>
+  <si>
+    <t>Q6 staż na 1 oddz.</t>
+  </si>
+  <si>
+    <t>Q7 wspierajace</t>
+  </si>
+  <si>
+    <t>Q9 syst. motyw.</t>
+  </si>
+  <si>
+    <t>Q10 do domu emocje</t>
+  </si>
+  <si>
+    <t>Q11 traumatyzacja</t>
+  </si>
+  <si>
+    <t>Q12 potrtafi niwelowac</t>
+  </si>
+  <si>
+    <t>Q13 używki</t>
+  </si>
+  <si>
+    <t>Q14 dylemat rozwoj</t>
+  </si>
+  <si>
+    <t>Q15 presja społeczna</t>
+  </si>
+  <si>
+    <t>Q16 doswiad. przemocy</t>
+  </si>
+  <si>
+    <t>Q17 post. dochodz.</t>
+  </si>
+  <si>
+    <t>Q18 bezp. covid</t>
+  </si>
+  <si>
+    <t>Q19 popiera strajki</t>
+  </si>
+  <si>
+    <t>Q20 satys. autonomi</t>
+  </si>
+  <si>
+    <t>Q21 kompetencje</t>
+  </si>
+  <si>
+    <t>Q22 potrz. psychologa</t>
+  </si>
+  <si>
+    <t>Q23 posiada pasje</t>
+  </si>
+  <si>
+    <t>Q24 uczest w życiu</t>
+  </si>
+  <si>
+    <t>Q25 partner w SOZ</t>
+  </si>
+  <si>
+    <t>Q26 rodzina wspiera</t>
+  </si>
+  <si>
+    <t>Q27 konflikt</t>
+  </si>
+  <si>
+    <t>Q28 praca pow niezgody</t>
+  </si>
+  <si>
+    <t>Q29 rozpad związku</t>
+  </si>
+  <si>
+    <t>Q30 rozważ. rezygnację</t>
+  </si>
+  <si>
+    <t>Q31 pracuje mimo ch.</t>
+  </si>
+  <si>
+    <t>Q32 korzysta ZLA</t>
+  </si>
+  <si>
+    <t>Q33 choruje</t>
+  </si>
+  <si>
+    <t>Q34 empatia</t>
+  </si>
+  <si>
+    <t>Q35 wypal. zawod.</t>
+  </si>
+  <si>
+    <t>Q36 dobry wybór</t>
+  </si>
+  <si>
+    <t>Q37 dziecko piel.</t>
+  </si>
+  <si>
+    <t>Q37</t>
   </si>
 </sst>
 </file>
@@ -580,8 +700,8 @@
   </sheetPr>
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR2" sqref="AR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,12 +837,12 @@
         <v>41</v>
       </c>
       <c r="AR1" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -820,7 +940,7 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
@@ -870,7 +990,7 @@
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
@@ -920,7 +1040,7 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
@@ -1022,7 +1142,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
@@ -1076,7 +1196,7 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1124,7 +1244,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2">
         <v>0.4</v>
@@ -1176,7 +1296,7 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2">
         <v>0.3</v>
@@ -1228,7 +1348,7 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1276,7 +1396,7 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2">
         <v>-0.2</v>
@@ -1334,7 +1454,7 @@
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1438,7 +1558,7 @@
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1488,7 +1608,7 @@
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1542,7 +1662,7 @@
     </row>
     <row r="18" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1594,7 +1714,7 @@
     </row>
     <row r="19" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1648,7 +1768,7 @@
     </row>
     <row r="20" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1702,7 +1822,7 @@
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1758,7 +1878,7 @@
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1822,7 +1942,7 @@
     </row>
     <row r="23" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2">
@@ -1882,7 +2002,7 @@
     </row>
     <row r="24" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1930,7 +2050,7 @@
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1992,7 +2112,7 @@
     </row>
     <row r="26" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2044,7 +2164,7 @@
     </row>
     <row r="27" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2098,7 +2218,7 @@
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2150,7 +2270,7 @@
     </row>
     <row r="29" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2210,7 +2330,7 @@
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2264,7 +2384,7 @@
     </row>
     <row r="31" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2326,7 +2446,7 @@
     </row>
     <row r="32" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2374,7 +2494,7 @@
     </row>
     <row r="33" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2428,7 +2548,7 @@
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2486,7 +2606,7 @@
     </row>
     <row r="35" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2554,7 +2674,7 @@
     </row>
     <row r="36" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2608,7 +2728,7 @@
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2">
@@ -2688,7 +2808,7 @@
     </row>
     <row r="38" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2752,7 +2872,7 @@
     </row>
     <row r="39" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2814,7 +2934,7 @@
     </row>
     <row r="40" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2872,7 +2992,7 @@
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2926,7 +3046,7 @@
     </row>
     <row r="42" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2">
@@ -3010,7 +3130,7 @@
     </row>
     <row r="43" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3080,7 +3200,7 @@
     </row>
     <row r="44" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2">

</xml_diff>